<commit_message>
In order to support Kempston mouse, addresses, address updated to A0=1, A1=1, A5=1, A7=0. This changes decoding bit from A6 to A5. Update #5
</commit_message>
<xml_diff>
--- a/address_analysis.xlsx
+++ b/address_analysis.xlsx
@@ -25,51 +25,55 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="K17" authorId="0">
+    <comment ref="K20" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Avoids conflict with Timex 2068. TBC.</t>
         </r>
       </text>
     </comment>
-    <comment ref="L17" authorId="0">
+    <comment ref="M20" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Avoids conflict with Kempston joystick (which we also emulate)
+          <t xml:space="preserve">Avoids conflict with Kempston joystick and mouse (which we also emulate)
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="Q17" authorId="0">
+    <comment ref="Q20" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Avoids conflict with 128/+2/+3 internal devices
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="R17" authorId="0">
+    <comment ref="R20" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Avoids conflict with Spectrum 
 ULA</t>
@@ -81,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="16">
   <si>
     <t xml:space="preserve">ULA</t>
   </si>
@@ -112,6 +116,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+3 FDC </t>
     </r>
@@ -121,6 +126,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -129,6 +135,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Status</t>
     </r>
@@ -138,12 +145,19 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Kempston </t>
+    <t xml:space="preserve">Kempston mouse X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kempston mouse buttons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kempston joystick</t>
   </si>
   <si>
     <t xml:space="preserve">ULA TS2068</t>
@@ -170,6 +184,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -191,6 +206,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -247,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,10 +289,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,13 +369,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:R43"/>
+  <dimension ref="B1:R46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U8" activeCellId="0" sqref="U8"/>
+      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="3" style="0" width="2.55"/>
@@ -838,20 +850,20 @@
       <c r="G10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2" t="n">
-        <v>0</v>
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="M10" s="2" t="n">
         <v>0</v>
@@ -874,7 +886,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1</v>
@@ -891,43 +903,43 @@
       <c r="G11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" s="2" t="n">
+      <c r="H11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R11" s="2" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1</v>
@@ -947,34 +959,34 @@
       <c r="H12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="2" t="n">
+      <c r="I12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1007,28 +1019,28 @@
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R13" s="2" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,21 +1084,21 @@
         <v>1</v>
       </c>
       <c r="O14" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="Q14" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="4" t="s">
-        <v>12</v>
+      <c r="B15" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>1</v>
@@ -1125,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="O15" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15" s="2" t="n">
         <v>1</v>
@@ -1134,30 +1146,65 @@
         <v>1</v>
       </c>
       <c r="R15" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5" t="s">
-        <v>13</v>
+      <c r="B17" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
@@ -1183,48 +1230,83 @@
       <c r="J17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="R17" s="6" t="n">
+      <c r="K17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="2"/>
@@ -1245,22 +1327,57 @@
       <c r="R19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M20" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R20" s="6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="2"/>
@@ -1676,6 +1793,60 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
     </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>